<commit_message>
Final version using input
</commit_message>
<xml_diff>
--- a/meals_overview_2024.xlsx
+++ b/meals_overview_2024.xlsx
@@ -1,47 +1,127 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vippsas-my.sharepoint.com/personal/nam_mai_vipps_no/Documents/Desktop/Temp/Pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_D17A7DC68E31D5F15BC7683911EBC6C2D742881A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC17BCBE-D522-FF4E-9EEC-416CF6DEAC79}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_71FCE7CE7D029340843D7546E16C652C9AC54E68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFBD217-05F9-2D45-B67E-6A40567A392F}"/>
   <bookViews>
-    <workbookView xWindow="21580" yWindow="3040" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="2980" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Oversikt måltider" sheetId="4" r:id="rId1"/>
-    <sheet name="TUNCO AS 01012024  30052024" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TUNCO AS 01012024  30052024" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="48">
   <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Sum of Antall</t>
+  </si>
+  <si>
+    <t>Meal amounts in kr</t>
+  </si>
+  <si>
+    <t>Total number of meals</t>
+  </si>
+  <si>
+    <t>Aira Ambrozaityte</t>
+  </si>
+  <si>
+    <t>Aliz Voloscsuk</t>
+  </si>
+  <si>
+    <t>Anamol  Raj Bhandari</t>
+  </si>
+  <si>
+    <t>Bernjard David Ruiz</t>
+  </si>
+  <si>
+    <t>Chelsea  Angelica Ryen</t>
+  </si>
+  <si>
+    <t>Christian Lothar Ruiz</t>
+  </si>
+  <si>
+    <t>Ella Rief</t>
+  </si>
+  <si>
+    <t>Elvis  Hito</t>
+  </si>
+  <si>
+    <t>Francisco Braga</t>
+  </si>
+  <si>
+    <t>Gonzalo  de Paul</t>
+  </si>
+  <si>
+    <t>Hadgu Hisabu</t>
+  </si>
+  <si>
+    <t>Iris  Lameiro Lopes</t>
+  </si>
+  <si>
+    <t>Isabelle Marty Bye</t>
+  </si>
+  <si>
+    <t>Jan Rosendahl</t>
+  </si>
+  <si>
+    <t>Joao Carlos  Gama dos Santos</t>
+  </si>
+  <si>
+    <t>Katarzyna Slysz</t>
+  </si>
+  <si>
+    <t>Kaung  Htet Aung</t>
+  </si>
+  <si>
+    <t>Laureano Orneles de Souza Júnior</t>
+  </si>
+  <si>
+    <t>Leonie Havens</t>
+  </si>
+  <si>
+    <t>Maria  Mangmee Solberg</t>
+  </si>
+  <si>
+    <t>Martin  Haláček</t>
+  </si>
+  <si>
+    <t>Martinho  Nora</t>
+  </si>
+  <si>
+    <t>Mateusz Tadeusz</t>
+  </si>
+  <si>
+    <t>Sebastian Andrzej  Halama</t>
+  </si>
+  <si>
+    <t>Yann Alberto Rendón Zapata</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Ansattnavn</t>
+  </si>
+  <si>
     <t>Ansattnummer</t>
   </si>
   <si>
-    <t>Ansattnavn</t>
-  </si>
-  <si>
     <t>Shiftnavn</t>
   </si>
   <si>
@@ -57,9 +137,6 @@
     <t>Avdelingsnummer</t>
   </si>
   <si>
-    <t>Aira Ambrozaityte</t>
-  </si>
-  <si>
     <t>Vakter</t>
   </si>
   <si>
@@ -75,109 +152,19 @@
     <t>Overtid over 80 timer per 2 uker</t>
   </si>
   <si>
-    <t>Aliz Voloscsuk</t>
-  </si>
-  <si>
-    <t>Anamol  Raj Bhandari</t>
-  </si>
-  <si>
     <t>André Evju</t>
   </si>
   <si>
     <t>Månedslønn</t>
   </si>
   <si>
-    <t>Bernjard David Ruiz</t>
-  </si>
-  <si>
-    <t>Chelsea  Angelica Ryen</t>
-  </si>
-  <si>
     <t>Egenmelding timelønn</t>
   </si>
   <si>
-    <t>Christian Lothar Ruiz</t>
-  </si>
-  <si>
-    <t>Ella Rief</t>
-  </si>
-  <si>
-    <t>Elvis  Hito</t>
-  </si>
-  <si>
-    <t>Francisco Braga</t>
-  </si>
-  <si>
-    <t>Gonzalo  de Paul</t>
-  </si>
-  <si>
-    <t>Hadgu Hisabu</t>
-  </si>
-  <si>
     <t>2,3,4</t>
   </si>
   <si>
-    <t>Iris  Lameiro Lopes</t>
-  </si>
-  <si>
-    <t>Isabelle Marty Bye</t>
-  </si>
-  <si>
-    <t>Jan Rosendahl</t>
-  </si>
-  <si>
-    <t>Joao Carlos  Gama dos Santos</t>
-  </si>
-  <si>
-    <t>Katarzyna Slysz</t>
-  </si>
-  <si>
-    <t>Kaung  Htet Aung</t>
-  </si>
-  <si>
-    <t>Laureano Orneles de Souza Júnior</t>
-  </si>
-  <si>
-    <t>Leonie Havens</t>
-  </si>
-  <si>
-    <t>Maria  Mangmee Solberg</t>
-  </si>
-  <si>
     <t>Maria Helena  Vesselinova Lakselvhaug</t>
-  </si>
-  <si>
-    <t>Martin  Haláček</t>
-  </si>
-  <si>
-    <t>Martinho  Nora</t>
-  </si>
-  <si>
-    <t>Mateusz Tadeusz</t>
-  </si>
-  <si>
-    <t>Sebastian Andrzej  Halama</t>
-  </si>
-  <si>
-    <t>Yann Alberto Rendón Zapata</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Sum of Antall</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Meal amounts in kr</t>
-  </si>
-  <si>
-    <t>Total number of meals</t>
-  </si>
-  <si>
-    <t>Employee ID</t>
   </si>
 </sst>
 </file>
@@ -217,7 +204,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -549,38 +536,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46945D89-FB26-9C46-8CF1-668B9EA95037}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="10.83203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="6" max="8" width="10.83203125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="F1" s="5">
         <v>45444</v>
@@ -591,7 +579,7 @@
         <v>1023</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6">
         <v>437.52</v>
@@ -611,7 +599,7 @@
         <v>1070</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6">
         <v>66.040000000000006</v>
@@ -631,7 +619,7 @@
         <v>1067</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" s="6">
         <v>109.32</v>
@@ -651,10 +639,10 @@
         <v>1063</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6">
-        <v>395.24999999999994</v>
+        <v>395.24999999999989</v>
       </c>
       <c r="D5" s="4">
         <v>1400</v>
@@ -671,7 +659,7 @@
         <v>1051</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C6" s="6">
         <v>224.73</v>
@@ -689,7 +677,7 @@
         <v>1064</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" s="6">
         <v>261.69</v>
@@ -709,7 +697,7 @@
         <v>1041</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6">
         <v>107.47</v>
@@ -729,7 +717,7 @@
         <v>1035</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6">
         <v>162.05000000000001</v>
@@ -749,7 +737,7 @@
         <v>1008</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6">
         <v>615.41999999999996</v>
@@ -769,7 +757,7 @@
         <v>1017</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C11" s="6">
         <v>277.5</v>
@@ -789,7 +777,7 @@
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6">
         <v>842.32</v>
@@ -809,7 +797,7 @@
         <v>1043</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6">
         <v>636.02</v>
@@ -829,7 +817,7 @@
         <v>1055</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C14" s="6">
         <v>13.35</v>
@@ -849,10 +837,10 @@
         <v>1059</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6">
-        <v>407.07000000000005</v>
+        <v>407.07000000000011</v>
       </c>
       <c r="D15" s="4">
         <v>1450</v>
@@ -869,7 +857,7 @@
         <v>1019</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <v>769.12</v>
@@ -889,7 +877,7 @@
         <v>1066</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C17" s="6">
         <v>94.45</v>
@@ -909,10 +897,10 @@
         <v>1045</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C18" s="6">
-        <v>442.19999999999993</v>
+        <v>442.19999999999987</v>
       </c>
       <c r="D18" s="4">
         <v>1600</v>
@@ -929,7 +917,7 @@
         <v>1056</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C19" s="6">
         <v>447.63</v>
@@ -949,7 +937,7 @@
         <v>1057</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C20" s="6">
         <v>587.26</v>
@@ -969,7 +957,7 @@
         <v>1062</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C21" s="6">
         <v>244.14</v>
@@ -989,7 +977,7 @@
         <v>1060</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C22" s="6">
         <v>574.04</v>
@@ -1009,7 +997,7 @@
         <v>1037</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C23" s="6">
         <v>436.27</v>
@@ -1029,10 +1017,10 @@
         <v>1068</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C24" s="6">
-        <v>100.86000000000001</v>
+        <v>100.86</v>
       </c>
       <c r="D24" s="4">
         <v>350</v>
@@ -1049,7 +1037,7 @@
         <v>1071</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C25" s="6">
         <v>83.45</v>
@@ -1069,7 +1057,7 @@
         <v>1069</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C26" s="6">
         <v>181.6</v>
@@ -1086,7 +1074,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3">
         <v>8523.8200000000015</v>
@@ -1108,10 +1096,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView topLeftCell="CE84" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1128,36 +1116,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1023</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>160.37</v>
@@ -1171,13 +1159,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1023</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>200.8</v>
@@ -1191,13 +1179,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1023</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>76.349999999999994</v>
@@ -1211,13 +1199,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1023</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>39.5</v>
@@ -1231,13 +1219,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>1023</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>14</v>
@@ -1251,7 +1239,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1023</v>
@@ -1265,13 +1253,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>1023</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>7.63</v>
@@ -1285,13 +1273,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1023</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>7.85</v>
@@ -1305,13 +1293,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>1023</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>3.98</v>
@@ -1325,13 +1313,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>1023</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>1.27</v>
@@ -1345,13 +1333,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>1070</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>40.92</v>
@@ -1365,13 +1353,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>1070</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>25.12</v>
@@ -1385,13 +1373,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>1070</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>7.52</v>
@@ -1405,13 +1393,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>1067</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>18.77</v>
@@ -1425,13 +1413,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>1067</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>34.369999999999997</v>
@@ -1445,13 +1433,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>1067</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>56.18</v>
@@ -1465,13 +1453,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1482,13 +1470,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>1063</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>27.2</v>
@@ -1502,13 +1490,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>1063</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>287.27999999999997</v>
@@ -1522,13 +1510,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>1063</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>80.77</v>
@@ -1542,7 +1530,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>1063</v>
@@ -1556,13 +1544,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>1063</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>6.15</v>
@@ -1576,13 +1564,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>1051</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>68.78</v>
@@ -1596,13 +1584,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>1051</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D25">
         <v>149.97999999999999</v>
@@ -1616,13 +1604,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>1051</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>5.97</v>
@@ -1636,13 +1624,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>1051</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -1656,13 +1644,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B28">
         <v>1051</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>6</v>
@@ -1676,13 +1664,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B29">
         <v>1051</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>6.03</v>
@@ -1696,13 +1684,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>1064</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D30">
         <v>201.17</v>
@@ -1716,13 +1704,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>1064</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D31">
         <v>34.97</v>
@@ -1736,13 +1724,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>1064</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D32">
         <v>25.55</v>
@@ -1756,7 +1744,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>1064</v>
@@ -1770,13 +1758,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B34">
         <v>1041</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D34">
         <v>62.42</v>
@@ -1790,13 +1778,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>1041</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <v>39.17</v>
@@ -1810,13 +1798,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>1041</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D36">
         <v>5.88</v>
@@ -1830,13 +1818,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>1041</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -1850,13 +1838,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B38">
         <v>1035</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D38">
         <v>162.05000000000001</v>
@@ -1870,7 +1858,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B39">
         <v>1035</v>
@@ -1884,13 +1872,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>1008</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>615.41999999999996</v>
@@ -1904,7 +1892,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>1008</v>
@@ -1918,13 +1906,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>1008</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D42">
         <v>7.5</v>
@@ -1938,13 +1926,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B43">
         <v>1017</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D43">
         <v>277.5</v>
@@ -1958,13 +1946,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B44">
         <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D44">
         <v>264.10000000000002</v>
@@ -1978,13 +1966,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B45">
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D45">
         <v>560.52</v>
@@ -1998,13 +1986,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B46">
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D46">
         <v>17.7</v>
@@ -2018,13 +2006,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B47">
         <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D47">
         <v>7.67</v>
@@ -2038,13 +2026,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B48">
         <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D48">
         <v>6.97</v>
@@ -2053,18 +2041,18 @@
         <v>89.19</v>
       </c>
       <c r="G48" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B49">
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D49">
         <v>6.73</v>
@@ -2078,13 +2066,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B50">
         <v>1043</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D50">
         <v>177.6</v>
@@ -2098,13 +2086,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B51">
         <v>1043</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D51">
         <v>10.75</v>
@@ -2118,13 +2106,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B52">
         <v>1043</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D52">
         <v>447.67</v>
@@ -2138,13 +2126,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B53">
         <v>1043</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D53">
         <v>7</v>
@@ -2158,7 +2146,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B54">
         <v>1043</v>
@@ -2172,13 +2160,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B55">
         <v>1043</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D55">
         <v>14.98</v>
@@ -2192,13 +2180,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B56">
         <v>1043</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D56">
         <v>18.78</v>
@@ -2212,13 +2200,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B57">
         <v>1043</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D57">
         <v>9.1300000000000008</v>
@@ -2232,13 +2220,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B58">
         <v>1055</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D58">
         <v>13.35</v>
@@ -2252,13 +2240,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B59">
         <v>1059</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D59">
         <v>128.53</v>
@@ -2272,13 +2260,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B60">
         <v>1059</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D60">
         <v>42.82</v>
@@ -2292,13 +2280,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B61">
         <v>1059</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D61">
         <v>171.37</v>
@@ -2312,13 +2300,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B62">
         <v>1059</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D62">
         <v>64.349999999999994</v>
@@ -2332,13 +2320,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B63">
         <v>1059</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D63">
         <v>12</v>
@@ -2352,13 +2340,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B64">
         <v>1019</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D64">
         <v>769.12</v>
@@ -2372,13 +2360,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B65">
         <v>1019</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D65">
         <v>7.5</v>
@@ -2392,13 +2380,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B66">
         <v>1019</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D66">
         <v>6.8</v>
@@ -2412,13 +2400,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B67">
         <v>1019</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D67">
         <v>17.03</v>
@@ -2432,13 +2420,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B68">
         <v>1019</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D68">
         <v>7.43</v>
@@ -2452,13 +2440,13 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B69">
         <v>1066</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D69">
         <v>64.03</v>
@@ -2472,13 +2460,13 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B70">
         <v>1066</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D70">
         <v>16.2</v>
@@ -2492,13 +2480,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B71">
         <v>1066</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D71">
         <v>14.22</v>
@@ -2512,13 +2500,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B72">
         <v>1066</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D72">
         <v>18</v>
@@ -2532,7 +2520,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B73">
         <v>1066</v>
@@ -2546,13 +2534,13 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B74">
         <v>1045</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D74">
         <v>312.52999999999997</v>
@@ -2566,13 +2554,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B75">
         <v>1045</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D75">
         <v>102.07</v>
@@ -2586,13 +2574,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B76">
         <v>1045</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D76">
         <v>27.6</v>
@@ -2606,13 +2594,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B77">
         <v>1045</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D77">
         <v>12</v>
@@ -2626,7 +2614,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B78">
         <v>1045</v>
@@ -2640,13 +2628,13 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B79">
         <v>1045</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D79">
         <v>6.28</v>
@@ -2660,13 +2648,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B80">
         <v>1045</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D80">
         <v>7.77</v>
@@ -2680,13 +2668,13 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B81">
         <v>1056</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D81">
         <v>360.3</v>
@@ -2700,13 +2688,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B82">
         <v>1056</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D82">
         <v>56.95</v>
@@ -2720,13 +2708,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B83">
         <v>1056</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D83">
         <v>30.38</v>
@@ -2740,13 +2728,13 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B84">
         <v>1056</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D84">
         <v>15</v>
@@ -2760,7 +2748,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B85">
         <v>1056</v>
@@ -2774,13 +2762,13 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B86">
         <v>1056</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D86">
         <v>5.23</v>
@@ -2794,13 +2782,13 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B87">
         <v>1057</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D87">
         <v>164.27</v>
@@ -2814,13 +2802,13 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B88">
         <v>1057</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D88">
         <v>415.42</v>
@@ -2834,13 +2822,13 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B89">
         <v>1057</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D89">
         <v>7.57</v>
@@ -2854,13 +2842,13 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B90">
         <v>1057</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D90">
         <v>22</v>
@@ -2874,7 +2862,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B91">
         <v>1057</v>
@@ -2888,13 +2876,13 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B92">
         <v>1057</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D92">
         <v>13.52</v>
@@ -2908,13 +2896,13 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B93">
         <v>1057</v>
       </c>
       <c r="C93" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D93">
         <v>0.15</v>
@@ -2928,13 +2916,13 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B94">
         <v>1057</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D94">
         <v>6.43</v>
@@ -2948,13 +2936,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B95">
         <v>1062</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D95">
         <v>180.47</v>
@@ -2968,13 +2956,13 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B96">
         <v>1062</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D96">
         <v>8.27</v>
@@ -2988,13 +2976,13 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B97">
         <v>1062</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D97">
         <v>35.450000000000003</v>
@@ -3008,13 +2996,13 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B98">
         <v>1062</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D98">
         <v>19.95</v>
@@ -3028,13 +3016,13 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B99">
         <v>1062</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D99">
         <v>8</v>
@@ -3048,13 +3036,13 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B100">
         <v>1062</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D100">
         <v>6.8</v>
@@ -3068,13 +3056,13 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B101">
         <v>100000000</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D101">
         <v>7.05</v>
@@ -3088,13 +3076,13 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B102">
         <v>1060</v>
       </c>
       <c r="C102" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D102">
         <v>16.97</v>
@@ -3108,13 +3096,13 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B103">
         <v>1060</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D103">
         <v>76.55</v>
@@ -3128,13 +3116,13 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B104">
         <v>1060</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D104">
         <v>473</v>
@@ -3148,13 +3136,13 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B105">
         <v>1060</v>
       </c>
       <c r="C105" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D105">
         <v>7.52</v>
@@ -3168,7 +3156,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B106">
         <v>1060</v>
@@ -3182,13 +3170,13 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B107">
         <v>1060</v>
       </c>
       <c r="C107" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D107">
         <v>15</v>
@@ -3202,13 +3190,13 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B108">
         <v>1060</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D108">
         <v>9.75</v>
@@ -3222,13 +3210,13 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B109">
         <v>1060</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D109">
         <v>4.18</v>
@@ -3242,13 +3230,13 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B110">
         <v>1037</v>
       </c>
       <c r="C110" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D110">
         <v>436.27</v>
@@ -3262,7 +3250,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B111">
         <v>1037</v>
@@ -3276,13 +3264,13 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B112">
         <v>1037</v>
       </c>
       <c r="C112" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D112">
         <v>7.52</v>
@@ -3296,13 +3284,13 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B113">
         <v>1068</v>
       </c>
       <c r="C113" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D113">
         <v>82.68</v>
@@ -3316,13 +3304,13 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B114">
         <v>1068</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D114">
         <v>4.03</v>
@@ -3336,13 +3324,13 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B115">
         <v>1068</v>
       </c>
       <c r="C115" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D115">
         <v>7.5</v>
@@ -3356,13 +3344,13 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B116">
         <v>1068</v>
       </c>
       <c r="C116" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D116">
         <v>6.65</v>
@@ -3376,13 +3364,13 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B117">
         <v>1068</v>
       </c>
       <c r="C117" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D117">
         <v>36</v>
@@ -3396,13 +3384,13 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B118">
         <v>1071</v>
       </c>
       <c r="C118" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D118">
         <v>7.73</v>
@@ -3416,13 +3404,13 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B119">
         <v>1071</v>
       </c>
       <c r="C119" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D119">
         <v>49.95</v>
@@ -3436,13 +3424,13 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B120">
         <v>1071</v>
       </c>
       <c r="C120" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D120">
         <v>4.5199999999999996</v>
@@ -3456,13 +3444,13 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B121">
         <v>1071</v>
       </c>
       <c r="C121" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D121">
         <v>21.25</v>
@@ -3476,7 +3464,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B122">
         <v>1071</v>
@@ -3490,13 +3478,13 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B123">
         <v>1071</v>
       </c>
       <c r="C123" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D123">
         <v>0.52</v>
@@ -3510,13 +3498,13 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B124">
         <v>1069</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D124">
         <v>20.52</v>
@@ -3530,13 +3518,13 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B125">
         <v>1069</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D125">
         <v>36.33</v>
@@ -3550,13 +3538,13 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B126">
         <v>1069</v>
       </c>
       <c r="C126" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D126">
         <v>109.9</v>
@@ -3570,13 +3558,13 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B127">
         <v>1069</v>
       </c>
       <c r="C127" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D127">
         <v>14.85</v>
@@ -3590,13 +3578,13 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B128">
         <v>1069</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D128">
         <v>7.12</v>
@@ -3610,13 +3598,13 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B129">
         <v>1069</v>
       </c>
       <c r="C129" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D129">
         <v>0.02</v>

</xml_diff>